<commit_message>
cleaned up the nib schematic
</commit_message>
<xml_diff>
--- a/nest_interface/eagle/rev_a/nest_interface_a_bom.xlsx
+++ b/nest_interface/eagle/rev_a/nest_interface_a_bom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="142">
   <si>
     <t>Quantity</t>
   </si>
@@ -34,6 +34,417 @@
   </si>
   <si>
     <t>Distributor</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>C-EUC0603</t>
+  </si>
+  <si>
+    <t>C0603</t>
+  </si>
+  <si>
+    <t>CAPACITOR, European symbol</t>
+  </si>
+  <si>
+    <t>INDUCTOR0603</t>
+  </si>
+  <si>
+    <t>L1, L2</t>
+  </si>
+  <si>
+    <t>Inductors</t>
+  </si>
+  <si>
+    <t>LED0603</t>
+  </si>
+  <si>
+    <t>LED-0603</t>
+  </si>
+  <si>
+    <t>LEDs</t>
+  </si>
+  <si>
+    <t>PINHD-2X10</t>
+  </si>
+  <si>
+    <t>2X10</t>
+  </si>
+  <si>
+    <t>PIN HEADER</t>
+  </si>
+  <si>
+    <t>SWITCH-SPSTPTH</t>
+  </si>
+  <si>
+    <t>SWITCH-SPDT</t>
+  </si>
+  <si>
+    <t>S1, S4</t>
+  </si>
+  <si>
+    <t>SPST Switch</t>
+  </si>
+  <si>
+    <t>0.1u</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>R-US_R0603</t>
+  </si>
+  <si>
+    <t>R0603</t>
+  </si>
+  <si>
+    <t>RESISTOR, American symbol</t>
+  </si>
+  <si>
+    <t>100k 0.1%</t>
+  </si>
+  <si>
+    <t>R76</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>R10, R11, R33, R35</t>
+  </si>
+  <si>
+    <t>10u</t>
+  </si>
+  <si>
+    <t>CAP_POL1206</t>
+  </si>
+  <si>
+    <t>EIA3216</t>
+  </si>
+  <si>
+    <t>C4, C15</t>
+  </si>
+  <si>
+    <t>Capacitor Polarized</t>
+  </si>
+  <si>
+    <t>1u</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>5.1M</t>
+  </si>
+  <si>
+    <t>R75</t>
+  </si>
+  <si>
+    <t>766161104GP</t>
+  </si>
+  <si>
+    <t>SOIC-16</t>
+  </si>
+  <si>
+    <t>RA5, RA6</t>
+  </si>
+  <si>
+    <t>ALD1107</t>
+  </si>
+  <si>
+    <t>SOIC-14</t>
+  </si>
+  <si>
+    <t>U8, U9, U10, U11</t>
+  </si>
+  <si>
+    <t>CONN_BLOCK_2</t>
+  </si>
+  <si>
+    <t>CONN_BLOCK_3</t>
+  </si>
+  <si>
+    <t>CONN_BLOCK_7</t>
+  </si>
+  <si>
+    <t>CONN_BLOCK_8</t>
+  </si>
+  <si>
+    <t>EPIC-CORE_A</t>
+  </si>
+  <si>
+    <t>EPIC-LCC68</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>EVQP2</t>
+  </si>
+  <si>
+    <t>S2, S3</t>
+  </si>
+  <si>
+    <t>FC-135_32.768KA-A3</t>
+  </si>
+  <si>
+    <t>FC-135</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>FT232RL</t>
+  </si>
+  <si>
+    <t>SSOP28</t>
+  </si>
+  <si>
+    <t>U1, U6</t>
+  </si>
+  <si>
+    <t>MMPQ2222A</t>
+  </si>
+  <si>
+    <t>QA1, QA2, QA3, QA4</t>
+  </si>
+  <si>
+    <t>MOLEX_MICRO_USB_B_047346</t>
+  </si>
+  <si>
+    <t>MPC1825</t>
+  </si>
+  <si>
+    <t>SOT-223-3</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>MSP430F1611IPM</t>
+  </si>
+  <si>
+    <t>PM/PAG64</t>
+  </si>
+  <si>
+    <t>U20</t>
+  </si>
+  <si>
+    <t>PCA9575</t>
+  </si>
+  <si>
+    <t>TSSOP28</t>
+  </si>
+  <si>
+    <t>U4, U5</t>
+  </si>
+  <si>
+    <t>PINH2X12</t>
+  </si>
+  <si>
+    <t>2X12</t>
+  </si>
+  <si>
+    <t>PJ-036A-SMT</t>
+  </si>
+  <si>
+    <t>PJ-0361-SMT</t>
+  </si>
+  <si>
+    <t>RT314524</t>
+  </si>
+  <si>
+    <t>S0418-CA</t>
+  </si>
+  <si>
+    <t>TC1262</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>VSSR1603103</t>
+  </si>
+  <si>
+    <t>LSSOP-16</t>
+  </si>
+  <si>
+    <t>RA7</t>
+  </si>
+  <si>
+    <t>VSSR2403103</t>
+  </si>
+  <si>
+    <t>LSSOP-24</t>
+  </si>
+  <si>
+    <t>RA1, RA2, RA4</t>
+  </si>
+  <si>
+    <t>DIGIKEY</t>
+  </si>
+  <si>
+    <t>MF MPN</t>
+  </si>
+  <si>
+    <t>OC_FARNELL</t>
+  </si>
+  <si>
+    <t>OC_NEWARK</t>
+  </si>
+  <si>
+    <t>C6, C7, C8, C9, C10, C11</t>
+  </si>
+  <si>
+    <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C5, C12, C13, C14, C17</t>
+  </si>
+  <si>
+    <t>R6, R7, R8, R9, R37, R38, R39, R66, R67, R72, R77</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4, R5, R73, R74, R78, R79, R80</t>
+  </si>
+  <si>
+    <t>15x 100k resistor array bussed</t>
+  </si>
+  <si>
+    <t>766-161-R100KP-ND</t>
+  </si>
+  <si>
+    <t>Source: http://www.ftdichip.com/Documents/DataSheets/DS_FT232R_v104.pdf</t>
+  </si>
+  <si>
+    <t>91K9918</t>
+  </si>
+  <si>
+    <t>4 npn transistor array</t>
+  </si>
+  <si>
+    <t>MMPQ2222ACT-ND</t>
+  </si>
+  <si>
+    <t>16 channel I2C GPIO module.</t>
+  </si>
+  <si>
+    <t>568-6647-1-ND</t>
+  </si>
+  <si>
+    <t>RE1, RE2, RE3, RE4, RE5, RE6</t>
+  </si>
+  <si>
+    <t>TC1262-5.0VDB-ND</t>
+  </si>
+  <si>
+    <t>12x 10k resistor array</t>
+  </si>
+  <si>
+    <t>VSSR24-10K-JI-ND</t>
+  </si>
+  <si>
+    <t>4x P-FET transistor chip</t>
+  </si>
+  <si>
+    <t>1014-1015-ND</t>
+  </si>
+  <si>
+    <t>2x 0.100 in screw terminal block</t>
+  </si>
+  <si>
+    <t>277-1273-ND</t>
+  </si>
+  <si>
+    <t>3x 0.100 in screw terminal block</t>
+  </si>
+  <si>
+    <t>277-1274-ND</t>
+  </si>
+  <si>
+    <t>7x 0.100 in screw terminal block</t>
+  </si>
+  <si>
+    <t>277-1278-ND</t>
+  </si>
+  <si>
+    <t>8x 0.100 in screw terminal block</t>
+  </si>
+  <si>
+    <t>277-1279-ND</t>
+  </si>
+  <si>
+    <t>MOLEX_MICRO_USB_B_</t>
+  </si>
+  <si>
+    <t>047346 MOLEX_MICRO_USB_B_047346</t>
+  </si>
+  <si>
+    <t>Very tiny smd micro USB receptacle.</t>
+  </si>
+  <si>
+    <t>WM17141CT-ND</t>
+  </si>
+  <si>
+    <t>3V 500mA LDO</t>
+  </si>
+  <si>
+    <t>MCP1825S-3002E/DB-ND</t>
+  </si>
+  <si>
+    <t>CONN PWR JACK 2.0X6.3MM SMT</t>
+  </si>
+  <si>
+    <t>CP-036APJCT-ND</t>
+  </si>
+  <si>
+    <t>RELAY GEN PURPOSE SPDT 16A 24VAC</t>
+  </si>
+  <si>
+    <t>PB1238-ND</t>
+  </si>
+  <si>
+    <t>5V 500mA LDO</t>
+  </si>
+  <si>
+    <t>RES ARRAY 10K OHM 8 RES 16-LSSOP</t>
+  </si>
+  <si>
+    <t>VSSR16-10K-JI-ND</t>
+  </si>
+  <si>
+    <t>j1, j2</t>
+  </si>
+  <si>
+    <t>j3</t>
+  </si>
+  <si>
+    <t>j4</t>
+  </si>
+  <si>
+    <t>j5</t>
+  </si>
+  <si>
+    <t>j6-j13</t>
+  </si>
+  <si>
+    <t>j14, j15</t>
+  </si>
+  <si>
+    <t>j18-j21</t>
+  </si>
+  <si>
+    <t>j16, j17</t>
   </si>
 </sst>
 </file>
@@ -402,15 +813,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="42.1640625" customWidth="1"/>
+    <col min="4" max="4" width="35.5" customWidth="1"/>
+    <col min="5" max="5" width="50.6640625" customWidth="1"/>
+    <col min="6" max="6" width="31.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,14 +844,756 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <f>LEN(B2)-LEN(SUBSTITUTE(B2,",",""))+1</f>
         <v>1</v>
       </c>
     </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>90</v>
+      </c>
+      <c r="H15" t="s">
+        <v>91</v>
+      </c>
+      <c r="I15" t="s">
+        <v>92</v>
+      </c>
+      <c r="J15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" t="s">
+        <v>134</v>
+      </c>
+      <c r="F21" t="s">
+        <v>123</v>
+      </c>
+      <c r="G21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" t="s">
+        <v>138</v>
+      </c>
+      <c r="F22" t="s">
+        <v>113</v>
+      </c>
+      <c r="G22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" t="s">
+        <v>139</v>
+      </c>
+      <c r="F23" t="s">
+        <v>115</v>
+      </c>
+      <c r="G23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" t="s">
+        <v>137</v>
+      </c>
+      <c r="F25" t="s">
+        <v>127</v>
+      </c>
+      <c r="G25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" t="s">
+        <v>140</v>
+      </c>
+      <c r="F26" t="s">
+        <v>119</v>
+      </c>
+      <c r="G26" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" t="s">
+        <v>141</v>
+      </c>
+      <c r="F27" t="s">
+        <v>117</v>
+      </c>
+      <c r="G27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" t="s">
+        <v>135</v>
+      </c>
+      <c r="F28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29">
+        <v>603</v>
+      </c>
+      <c r="E29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" t="s">
+        <v>65</v>
+      </c>
+      <c r="F30" t="s">
+        <v>103</v>
+      </c>
+      <c r="G30" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>240</v>
+      </c>
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" t="s">
+        <v>98</v>
+      </c>
+      <c r="F31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33">
+        <v>11</v>
+      </c>
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" t="s">
+        <v>97</v>
+      </c>
+      <c r="F33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" t="s">
+        <v>31</v>
+      </c>
+      <c r="F35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="B36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" t="s">
+        <v>88</v>
+      </c>
+      <c r="E36" t="s">
+        <v>89</v>
+      </c>
+      <c r="F36" t="s">
+        <v>109</v>
+      </c>
+      <c r="G36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37" t="s">
+        <v>99</v>
+      </c>
+      <c r="G37" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" t="s">
+        <v>85</v>
+      </c>
+      <c r="E38" t="s">
+        <v>86</v>
+      </c>
+      <c r="F38" t="s">
+        <v>132</v>
+      </c>
+      <c r="G38" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39">
+        <v>6</v>
+      </c>
+      <c r="B39" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" t="s">
+        <v>81</v>
+      </c>
+      <c r="E39" t="s">
+        <v>107</v>
+      </c>
+      <c r="F39" t="s">
+        <v>129</v>
+      </c>
+      <c r="G39" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" t="s">
+        <v>23</v>
+      </c>
+      <c r="F40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41">
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D42" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" t="s">
+        <v>63</v>
+      </c>
+      <c r="F42" t="s">
+        <v>101</v>
+      </c>
+      <c r="H42" t="s">
+        <v>61</v>
+      </c>
+      <c r="I42">
+        <v>1146032</v>
+      </c>
+      <c r="J42" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" t="s">
+        <v>53</v>
+      </c>
+      <c r="D43" t="s">
+        <v>54</v>
+      </c>
+      <c r="E43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" t="s">
+        <v>70</v>
+      </c>
+      <c r="D44" t="s">
+        <v>71</v>
+      </c>
+      <c r="E44" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C45" t="s">
+        <v>67</v>
+      </c>
+      <c r="D45" t="s">
+        <v>68</v>
+      </c>
+      <c r="E45" t="s">
+        <v>69</v>
+      </c>
+      <c r="F45" t="s">
+        <v>125</v>
+      </c>
+      <c r="G45" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="B46" t="s">
+        <v>73</v>
+      </c>
+      <c r="C46" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46" t="s">
+        <v>74</v>
+      </c>
+      <c r="E46" t="s">
+        <v>75</v>
+      </c>
+      <c r="F46" t="s">
+        <v>105</v>
+      </c>
+      <c r="G46" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" t="s">
+        <v>82</v>
+      </c>
+      <c r="D47" t="s">
+        <v>68</v>
+      </c>
+      <c r="E47" t="s">
+        <v>83</v>
+      </c>
+      <c r="F47" t="s">
+        <v>131</v>
+      </c>
+      <c r="G47" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48">
+        <v>4</v>
+      </c>
+      <c r="B48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" t="s">
+        <v>47</v>
+      </c>
+      <c r="E48" t="s">
+        <v>48</v>
+      </c>
+      <c r="F48" t="s">
+        <v>111</v>
+      </c>
+      <c r="G48" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" t="s">
+        <v>58</v>
+      </c>
+      <c r="D49" t="s">
+        <v>59</v>
+      </c>
+      <c r="E49" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A16:J49">
+    <sortCondition ref="E16:E49"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
added board for keypad socket
</commit_message>
<xml_diff>
--- a/nest_interface/eagle/rev_a/nest_interface_a_bom.xlsx
+++ b/nest_interface/eagle/rev_a/nest_interface_a_bom.xlsx
@@ -15,9 +15,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="142">
-  <si>
-    <t>Quantity</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="148">
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>Package</t>
   </si>
   <si>
     <t>Parts</t>
@@ -26,24 +35,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Part No.</t>
-  </si>
-  <si>
-    <t>Distributor</t>
-  </si>
-  <si>
-    <t>Package</t>
-  </si>
-  <si>
-    <t>Qty</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Device</t>
-  </si>
-  <si>
     <t>DIGIKEY</t>
   </si>
   <si>
@@ -56,7 +47,7 @@
     <t>C0603</t>
   </si>
   <si>
-    <t>C1, C2, C3, C4, C5, C6, C7, C8, C9, C10, C11, C12, C13, C14, C18, C19</t>
+    <t>C1, C2, C3, C4, C5, C6, C7, C8, C9, C10, C11, C12, C13, C14, C15, C16</t>
   </si>
   <si>
     <t>CAPACITOR, European symbol</t>
@@ -65,7 +56,7 @@
     <t>1u</t>
   </si>
   <si>
-    <t>C15</t>
+    <t>C17</t>
   </si>
   <si>
     <t>10u</t>
@@ -77,24 +68,42 @@
     <t>EIA3216</t>
   </si>
   <si>
-    <t>C16, C17</t>
+    <t>C18, C19</t>
   </si>
   <si>
     <t>Capacitor Polarized</t>
   </si>
   <si>
+    <t>478-1655-1-ND</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
     <t>LED0603</t>
   </si>
   <si>
     <t>LED-0603</t>
   </si>
   <si>
-    <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10</t>
+    <t>D1, D3, D6, D8</t>
   </si>
   <si>
     <t>LEDs</t>
   </si>
   <si>
+    <t>BLUE</t>
+  </si>
+  <si>
+    <t>D2, D5, D7, D10</t>
+  </si>
+  <si>
+    <t>GREEN</t>
+  </si>
+  <si>
+    <t>D4, D9</t>
+  </si>
+  <si>
     <t>MOLEX_MICRO_USB_B_047346</t>
   </si>
   <si>
@@ -203,6 +212,9 @@
     <t>Inductors</t>
   </si>
   <si>
+    <t>240-2373-1-ND</t>
+  </si>
+  <si>
     <t>TRANSISTOR_NPNSOT23</t>
   </si>
   <si>
@@ -362,6 +374,9 @@
     <t>S3, S4</t>
   </si>
   <si>
+    <t>P11084SCT-ND</t>
+  </si>
+  <si>
     <t>EPIC-CORE_A</t>
   </si>
   <si>
@@ -441,6 +456,9 @@
   </si>
   <si>
     <t>Y1</t>
+  </si>
+  <si>
+    <t>535-9543-1-ND</t>
   </si>
 </sst>
 </file>
@@ -516,11 +534,8 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -538,21 +553,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B22" activeCellId="0" pane="topLeft" sqref="B22"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B10" activeCellId="0" pane="topLeft" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.62352941176471"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.6392156862745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.843137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1647058823529"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="57.2627450980392"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.5921568627451"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.678431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.4980392156863"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.63137254901961"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.6588235294118"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8627450980392"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1725490196078"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="57.3019607843137"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.6117647058823"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.5058823529412"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="1">
@@ -574,612 +589,675 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
-        <f aca="false">LEN(B2)-LEN(SUBSTITUTE(B2,",",""))+1</f>
+        <v>16</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="B3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="4">
+      <c r="A4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="5">
-      <c r="A5" s="0" t="s">
-        <v>6</v>
+      <c r="A5" s="0" t="n">
+        <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="6">
       <c r="A6" s="0" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="7">
       <c r="A7" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="8">
+        <v>24</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="8">
       <c r="A8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>21</v>
+        <v>31</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="9">
       <c r="A9" s="0" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="10">
+        <v>36</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="10">
       <c r="A10" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="11">
       <c r="A11" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="B11" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="C11" s="0" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>33</v>
+        <v>43</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="12">
       <c r="A12" s="0" t="n">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>33</v>
+        <v>47</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="13">
       <c r="A13" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="14">
       <c r="A14" s="0" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="15">
       <c r="A15" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="16">
       <c r="A16" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>50</v>
-      </c>
       <c r="C16" s="0" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="17">
       <c r="A17" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="18">
+        <v>70</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="18">
       <c r="A18" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>71</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>61</v>
+        <v>74</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>75</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="19">
       <c r="A19" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>76</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="20">
+        <v>80</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="20">
       <c r="A20" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>67</v>
+        <v>10</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>240</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="21">
       <c r="A21" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="22">
       <c r="A22" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B22" s="1" t="n">
-        <v>240</v>
+        <v>1</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>87</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="23">
       <c r="A23" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="D23" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="24">
       <c r="A24" s="0" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E24" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="25">
       <c r="A25" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>80</v>
+        <v>96</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="26">
       <c r="A26" s="0" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>80</v>
+        <v>100</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>101</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="27">
       <c r="A27" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="28">
       <c r="A28" s="0" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="29">
       <c r="A29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>98</v>
+        <v>2</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="30">
       <c r="A30" s="0" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="F30" s="0" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="31">
       <c r="A31" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>120</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="G31" s="0" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="32">
       <c r="A32" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="33">
       <c r="A33" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>117</v>
+        <v>128</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>129</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="34">
@@ -1187,59 +1265,68 @@
         <v>1</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>120</v>
+        <v>132</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>134</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="35">
       <c r="A35" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>123</v>
+        <v>136</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>137</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="36">
       <c r="A36" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="37">
@@ -1247,68 +1334,25 @@
         <v>1</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="38">
-      <c r="A38" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="F38" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="G38" s="0" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="39">
-      <c r="A39" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.346527777777778" right="0.219444444444444" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>